<commit_message>
first major push to quarto repo
</commit_message>
<xml_diff>
--- a/data/toothpaste.xlsx
+++ b/data/toothpaste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://webmailbyui-my.sharepoint.com/personal/drp36_byui_edu/Documents/Math326DoE/Math326_Quarto4/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="8_{0DF32456-55C8-44A9-B7F7-2296BF79388F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3FAD757D-2E84-4B7E-A109-453EDF9962A5}"/>
+  <xr:revisionPtr revIDLastSave="267" documentId="8_{0DF32456-55C8-44A9-B7F7-2296BF79388F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E94A568-1709-4EDC-B2BD-94536E3816EB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="4" r:id="rId1"/>
@@ -18,10 +18,11 @@
     <sheet name="ToothbrushStudy_Data" sheetId="1" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId4"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId5"/>
+    <sheet name="Sheet4" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="144">
   <si>
     <t>Brush</t>
   </si>
@@ -217,12 +218,6 @@
   </si>
   <si>
     <t>Observations</t>
-  </si>
-  <si>
-    <t>means</t>
-  </si>
-  <si>
-    <t>effects</t>
   </si>
   <si>
     <t>=</t>
@@ -1098,15 +1093,126 @@
   <si>
     <t>Toothpaste Brand</t>
   </si>
+  <si>
+    <r>
+      <t>y</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ij</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>α</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ε</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ij</t>
+    </r>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>MSE</t>
+  </si>
+  <si>
+    <t>Mean of 3 values</t>
+  </si>
+  <si>
+    <t>free to vary</t>
+  </si>
+  <si>
+    <t>Depends on</t>
+  </si>
+  <si>
+    <t>the other 2</t>
+  </si>
+  <si>
+    <t>value1</t>
+  </si>
+  <si>
+    <t>value2</t>
+  </si>
+  <si>
+    <t>value3</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>3 x 10 - (a+b)</t>
+  </si>
+  <si>
+    <t>Brush Means</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>p-value</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Treatment Factor</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1312,6 +1418,27 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -1500,7 +1627,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -1876,6 +2003,55 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1922,7 +2098,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2001,9 +2177,6 @@
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="39" fontId="0" fillId="33" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2064,53 +2237,166 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="33" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="18" fillId="33" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="37" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="27" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="27" fillId="33" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="25" fillId="33" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="25" fillId="33" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="25" fillId="33" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="25" fillId="33" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="25" fillId="33" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="25" fillId="33" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="25" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="25" fillId="33" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="25" fillId="33" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="25" fillId="33" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="25" fillId="33" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="25" fillId="33" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="25" fillId="33" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="25" fillId="33" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="25" fillId="33" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="25" fillId="33" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="25" fillId="33" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="25" fillId="33" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="25" fillId="33" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="25" fillId="33" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="25" fillId="33" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2121,36 +2407,23 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="27" fillId="33" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="25" fillId="33" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="30" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2840,15 +3113,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Y40"/>
+  <dimension ref="A1:AC67"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:T18"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="J58" sqref="J58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="1" max="1" width="2.28515625" style="1" customWidth="1"/>
     <col min="2" max="4" width="7.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.28515625" style="1" customWidth="1"/>
     <col min="6" max="12" width="7.5703125" style="1" customWidth="1"/>
@@ -2856,18 +3129,25 @@
     <col min="14" max="14" width="6.42578125" style="1" customWidth="1"/>
     <col min="15" max="15" width="9" style="1" customWidth="1"/>
     <col min="16" max="20" width="7.5703125" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="1"/>
+    <col min="21" max="23" width="9.140625" style="1"/>
+    <col min="24" max="24" width="13.5703125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="6.85546875" style="1" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:29" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="K1" s="83"/>
+      <c r="L1" s="98" t="s">
+        <v>138</v>
+      </c>
+      <c r="M1" s="98"/>
+      <c r="N1" s="98"/>
+      <c r="O1" s="98"/>
+    </row>
+    <row r="2" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="18" t="s">
         <v>4</v>
       </c>
@@ -2880,20 +3160,44 @@
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="G2" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
+      <c r="L2" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="M2" s="82" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="N2" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="O2" s="82" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X2" s="56" t="s">
+        <v>124</v>
+      </c>
+      <c r="Y2" s="56" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z2" s="56" t="s">
+        <v>125</v>
+      </c>
+      <c r="AA2" s="56" t="s">
+        <v>139</v>
+      </c>
+      <c r="AB2" s="56" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC2" s="56" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>19.12</v>
       </c>
@@ -2906,24 +3210,55 @@
       <c r="E3" s="1">
         <v>24.39</v>
       </c>
-      <c r="H3" s="1">
-        <f>AVERAGE(B$3:B$8)</f>
+      <c r="G3" s="89">
+        <f>AVERAGE($B$13:$E$18)</f>
+        <v>22.764583333333331</v>
+      </c>
+      <c r="H3" s="90">
+        <f t="shared" ref="H3:J8" si="0">AVERAGE($B$13:$E$18)</f>
+        <v>22.764583333333331</v>
+      </c>
+      <c r="I3" s="90">
+        <f t="shared" si="0"/>
+        <v>22.764583333333331</v>
+      </c>
+      <c r="J3" s="91">
+        <f t="shared" si="0"/>
+        <v>22.764583333333331</v>
+      </c>
+      <c r="K3" s="57"/>
+      <c r="L3" s="84">
+        <f t="shared" ref="L3:O8" si="1">AVERAGE(B$3:B$8)</f>
         <v>23.093333333333334</v>
       </c>
-      <c r="I3" s="1">
-        <f t="shared" ref="I3:I8" si="0">AVERAGE(C$3:C$8)</f>
+      <c r="M3" s="84">
+        <f t="shared" si="1"/>
         <v>19.97666666666667</v>
       </c>
-      <c r="J3" s="1">
-        <f t="shared" ref="J3:J8" si="1">AVERAGE(D$3:D$8)</f>
+      <c r="N3" s="84">
+        <f t="shared" si="1"/>
         <v>22.675000000000001</v>
       </c>
-      <c r="K3" s="1">
-        <f t="shared" ref="K3:K8" si="2">AVERAGE(E$3:E$8)</f>
+      <c r="O3" s="87">
+        <f t="shared" si="1"/>
         <v>25.313333333333343</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="24">
+        <f>SUMSQ(G13:J18)</f>
+        <v>12437.430104166664</v>
+      </c>
+      <c r="AA3" s="24">
+        <f>Z3/Y3</f>
+        <v>12437.430104166664</v>
+      </c>
+    </row>
+    <row r="4" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>24.21</v>
       </c>
@@ -2936,24 +3271,59 @@
       <c r="E4" s="1">
         <v>21.45</v>
       </c>
-      <c r="H4" s="1">
-        <f t="shared" ref="H4:H8" si="3">AVERAGE(B$3:B$8)</f>
+      <c r="G4" s="92">
+        <f t="shared" ref="G4:G8" si="2">AVERAGE($B$13:$E$18)</f>
+        <v>22.764583333333331</v>
+      </c>
+      <c r="H4" s="38">
+        <f t="shared" si="0"/>
+        <v>22.764583333333331</v>
+      </c>
+      <c r="I4" s="38">
+        <f t="shared" si="0"/>
+        <v>22.764583333333331</v>
+      </c>
+      <c r="J4" s="87">
+        <f t="shared" si="0"/>
+        <v>22.764583333333331</v>
+      </c>
+      <c r="K4" s="57"/>
+      <c r="L4" s="85">
+        <f t="shared" si="1"/>
         <v>23.093333333333334</v>
       </c>
-      <c r="I4" s="1">
-        <f t="shared" si="0"/>
+      <c r="M4" s="85">
+        <f t="shared" si="1"/>
         <v>19.97666666666667</v>
       </c>
-      <c r="J4" s="1">
+      <c r="N4" s="85">
         <f t="shared" si="1"/>
         <v>22.675000000000001</v>
       </c>
-      <c r="K4" s="1">
-        <f t="shared" si="2"/>
+      <c r="O4" s="87">
+        <f t="shared" si="1"/>
         <v>25.313333333333343</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X4" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>3</v>
+      </c>
+      <c r="Z4" s="24">
+        <f>SUMSQ(L13:O18)</f>
+        <v>86.308245833333544</v>
+      </c>
+      <c r="AA4" s="24">
+        <f t="shared" ref="AA4:AA5" si="3">Z4/Y4</f>
+        <v>28.769415277777849</v>
+      </c>
+      <c r="AB4" s="24">
+        <f>AA4/AA5</f>
+        <v>3.8216608725476551</v>
+      </c>
+    </row>
+    <row r="5" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>26.88</v>
       </c>
@@ -2966,24 +3336,55 @@
       <c r="E5" s="1">
         <v>32.74</v>
       </c>
-      <c r="H5" s="1">
-        <f t="shared" si="3"/>
+      <c r="G5" s="92">
+        <f t="shared" si="2"/>
+        <v>22.764583333333331</v>
+      </c>
+      <c r="H5" s="38">
+        <f t="shared" si="0"/>
+        <v>22.764583333333331</v>
+      </c>
+      <c r="I5" s="38">
+        <f t="shared" si="0"/>
+        <v>22.764583333333331</v>
+      </c>
+      <c r="J5" s="87">
+        <f t="shared" si="0"/>
+        <v>22.764583333333331</v>
+      </c>
+      <c r="K5" s="57"/>
+      <c r="L5" s="85">
+        <f t="shared" si="1"/>
         <v>23.093333333333334</v>
       </c>
-      <c r="I5" s="1">
-        <f t="shared" si="0"/>
+      <c r="M5" s="85">
+        <f t="shared" si="1"/>
         <v>19.97666666666667</v>
       </c>
-      <c r="J5" s="1">
+      <c r="N5" s="85">
         <f t="shared" si="1"/>
         <v>22.675000000000001</v>
       </c>
-      <c r="K5" s="1">
-        <f t="shared" si="2"/>
+      <c r="O5" s="87">
+        <f t="shared" si="1"/>
         <v>25.313333333333343</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>20</v>
+      </c>
+      <c r="Z5" s="24">
+        <f>SUMSQ(Q13:T18)</f>
+        <v>150.55975000000004</v>
+      </c>
+      <c r="AA5" s="24">
+        <f t="shared" si="3"/>
+        <v>7.5279875000000018</v>
+      </c>
+    </row>
+    <row r="6" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>21.6</v>
       </c>
@@ -2996,24 +3397,51 @@
       <c r="E6" s="1">
         <v>24.21</v>
       </c>
-      <c r="H6" s="1">
-        <f t="shared" si="3"/>
+      <c r="G6" s="92">
+        <f t="shared" si="2"/>
+        <v>22.764583333333331</v>
+      </c>
+      <c r="H6" s="38">
+        <f t="shared" si="0"/>
+        <v>22.764583333333331</v>
+      </c>
+      <c r="I6" s="38">
+        <f t="shared" si="0"/>
+        <v>22.764583333333331</v>
+      </c>
+      <c r="J6" s="87">
+        <f t="shared" si="0"/>
+        <v>22.764583333333331</v>
+      </c>
+      <c r="K6" s="57"/>
+      <c r="L6" s="85">
+        <f t="shared" si="1"/>
         <v>23.093333333333334</v>
       </c>
-      <c r="I6" s="1">
-        <f t="shared" si="0"/>
+      <c r="M6" s="85">
+        <f t="shared" si="1"/>
         <v>19.97666666666667</v>
       </c>
-      <c r="J6" s="1">
+      <c r="N6" s="85">
         <f t="shared" si="1"/>
         <v>22.675000000000001</v>
       </c>
-      <c r="K6" s="1">
-        <f t="shared" si="2"/>
+      <c r="O6" s="87">
+        <f t="shared" si="1"/>
         <v>25.313333333333343</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X6" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>24</v>
+      </c>
+      <c r="Z6" s="24">
+        <f>SUMSQ(B3:E8)</f>
+        <v>12674.298100000002</v>
+      </c>
+    </row>
+    <row r="7" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>23.4</v>
       </c>
@@ -3026,24 +3454,41 @@
       <c r="E7" s="1">
         <v>25.67</v>
       </c>
-      <c r="H7" s="1">
-        <f t="shared" si="3"/>
+      <c r="G7" s="92">
+        <f t="shared" si="2"/>
+        <v>22.764583333333331</v>
+      </c>
+      <c r="H7" s="38">
+        <f t="shared" si="0"/>
+        <v>22.764583333333331</v>
+      </c>
+      <c r="I7" s="38">
+        <f t="shared" si="0"/>
+        <v>22.764583333333331</v>
+      </c>
+      <c r="J7" s="87">
+        <f t="shared" si="0"/>
+        <v>22.764583333333331</v>
+      </c>
+      <c r="K7" s="57"/>
+      <c r="L7" s="85">
+        <f t="shared" si="1"/>
         <v>23.093333333333334</v>
       </c>
-      <c r="I7" s="1">
-        <f t="shared" si="0"/>
+      <c r="M7" s="85">
+        <f t="shared" si="1"/>
         <v>19.97666666666667</v>
       </c>
-      <c r="J7" s="1">
+      <c r="N7" s="85">
         <f t="shared" si="1"/>
         <v>22.675000000000001</v>
       </c>
-      <c r="K7" s="1">
-        <f t="shared" si="2"/>
+      <c r="O7" s="87">
+        <f t="shared" si="1"/>
         <v>25.313333333333343</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>23.35</v>
       </c>
@@ -3056,40 +3501,59 @@
       <c r="E8" s="1">
         <v>23.42</v>
       </c>
-      <c r="H8" s="1">
-        <f t="shared" si="3"/>
+      <c r="G8" s="93">
+        <f t="shared" si="2"/>
+        <v>22.764583333333331</v>
+      </c>
+      <c r="H8" s="94">
+        <f t="shared" si="0"/>
+        <v>22.764583333333331</v>
+      </c>
+      <c r="I8" s="94">
+        <f t="shared" si="0"/>
+        <v>22.764583333333331</v>
+      </c>
+      <c r="J8" s="88">
+        <f t="shared" si="0"/>
+        <v>22.764583333333331</v>
+      </c>
+      <c r="K8" s="57"/>
+      <c r="L8" s="86">
+        <f t="shared" si="1"/>
         <v>23.093333333333334</v>
       </c>
-      <c r="I8" s="1">
-        <f t="shared" si="0"/>
+      <c r="M8" s="86">
+        <f t="shared" si="1"/>
         <v>19.97666666666667</v>
       </c>
-      <c r="J8" s="1">
+      <c r="N8" s="86">
         <f t="shared" si="1"/>
         <v>22.675000000000001</v>
       </c>
-      <c r="K8" s="1">
-        <f t="shared" si="2"/>
+      <c r="O8" s="88">
+        <f t="shared" si="1"/>
         <v>25.313333333333343</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Z8" s="97"/>
+    </row>
+    <row r="10" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="Z10" s="1">
+        <f>12437.43+86.31+150.56</f>
+        <v>12674.3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:29" x14ac:dyDescent="0.25">
       <c r="C11" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="L11" s="57" t="s">
-        <v>63</v>
-      </c>
-      <c r="M11" s="57"/>
-      <c r="N11" s="57"/>
-      <c r="O11" s="57"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="L11" s="98" t="s">
+        <v>61</v>
+      </c>
+      <c r="M11" s="98"/>
+      <c r="N11" s="98"/>
+      <c r="O11" s="98"/>
+    </row>
+    <row r="12" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
         <v>4</v>
       </c>
@@ -3102,12 +3566,12 @@
       <c r="E12" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G12" s="59" t="s">
+      <c r="G12" s="114" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="59"/>
-      <c r="I12" s="59"/>
-      <c r="J12" s="59"/>
+      <c r="H12" s="114"/>
+      <c r="I12" s="114"/>
+      <c r="J12" s="114"/>
       <c r="L12" s="18" t="s">
         <v>4</v>
       </c>
@@ -3120,14 +3584,14 @@
       <c r="O12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q12" s="59" t="s">
+      <c r="Q12" s="114" t="s">
         <v>48</v>
       </c>
-      <c r="R12" s="59"/>
-      <c r="S12" s="59"/>
-      <c r="T12" s="59"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R12" s="114"/>
+      <c r="S12" s="114"/>
+      <c r="T12" s="114"/>
+    </row>
+    <row r="13" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B13" s="18">
         <v>19.12</v>
       </c>
@@ -3140,58 +3604,58 @@
       <c r="E13" s="18">
         <v>24.39</v>
       </c>
-      <c r="G13" s="40">
+      <c r="G13" s="39">
         <f>AVERAGE($B$13:$E$18)</f>
         <v>22.764583333333331</v>
       </c>
-      <c r="H13" s="41">
+      <c r="H13" s="40">
         <f t="shared" ref="H13:J18" si="4">AVERAGE($B$13:$E$18)</f>
         <v>22.764583333333331</v>
       </c>
-      <c r="I13" s="41">
+      <c r="I13" s="40">
         <f t="shared" si="4"/>
         <v>22.764583333333331</v>
       </c>
-      <c r="J13" s="42">
+      <c r="J13" s="41">
         <f t="shared" si="4"/>
         <v>22.764583333333331</v>
       </c>
       <c r="K13" s="18"/>
-      <c r="L13" s="49">
-        <f>H3-$H$13</f>
+      <c r="L13" s="75">
+        <f t="shared" ref="L13:O18" si="5">L3-$H$13</f>
         <v>0.32875000000000298</v>
       </c>
-      <c r="M13" s="49">
-        <f t="shared" ref="M13:O13" si="5">I3-$H$13</f>
+      <c r="M13" s="75">
+        <f t="shared" si="5"/>
         <v>-2.7879166666666606</v>
       </c>
-      <c r="N13" s="49">
+      <c r="N13" s="75">
         <f t="shared" si="5"/>
         <v>-8.9583333333330017E-2</v>
       </c>
-      <c r="O13" s="49">
+      <c r="O13" s="75">
         <f t="shared" si="5"/>
         <v>2.5487500000000125</v>
       </c>
       <c r="P13" s="18"/>
-      <c r="Q13" s="36">
+      <c r="Q13" s="70">
         <f>B13-(G13+L13)</f>
         <v>-3.9733333333333327</v>
       </c>
-      <c r="R13" s="36">
+      <c r="R13" s="70">
         <f t="shared" ref="R13:R18" si="6">C13-(H13+M13)</f>
         <v>-1.4166666666666714</v>
       </c>
-      <c r="S13" s="36">
+      <c r="S13" s="70">
         <f t="shared" ref="S13:S18" si="7">D13-(I13+N13)</f>
         <v>2.9049999999999976</v>
       </c>
-      <c r="T13" s="36">
+      <c r="T13" s="70">
         <f t="shared" ref="T13:T18" si="8">E13-(J13+O13)</f>
         <v>-0.92333333333334267</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B14" s="18">
         <v>24.21</v>
       </c>
@@ -3204,58 +3668,62 @@
       <c r="E14" s="18">
         <v>21.45</v>
       </c>
-      <c r="G14" s="45">
+      <c r="G14" s="44">
         <f t="shared" ref="G14:G18" si="9">AVERAGE($B$13:$E$18)</f>
         <v>22.764583333333331</v>
       </c>
-      <c r="H14" s="39">
+      <c r="H14" s="38">
         <f t="shared" si="4"/>
         <v>22.764583333333331</v>
       </c>
-      <c r="I14" s="39">
+      <c r="I14" s="38">
         <f t="shared" si="4"/>
         <v>22.764583333333331</v>
       </c>
-      <c r="J14" s="44">
+      <c r="J14" s="43">
         <f t="shared" si="4"/>
         <v>22.764583333333331</v>
       </c>
       <c r="K14" s="18"/>
-      <c r="L14" s="51">
-        <f t="shared" ref="L14:L18" si="10">H4-$H$13</f>
+      <c r="L14" s="95">
+        <f t="shared" si="5"/>
         <v>0.32875000000000298</v>
       </c>
-      <c r="M14" s="51">
-        <f t="shared" ref="M14:M18" si="11">I4-$H$13</f>
+      <c r="M14" s="95">
+        <f t="shared" si="5"/>
         <v>-2.7879166666666606</v>
       </c>
-      <c r="N14" s="51">
-        <f t="shared" ref="N14:N18" si="12">J4-$H$13</f>
+      <c r="N14" s="95">
+        <f t="shared" si="5"/>
         <v>-8.9583333333330017E-2</v>
       </c>
-      <c r="O14" s="51">
-        <f t="shared" ref="O14:O18" si="13">K4-$H$13</f>
+      <c r="O14" s="95">
+        <f t="shared" si="5"/>
         <v>2.5487500000000125</v>
       </c>
       <c r="P14" s="18"/>
-      <c r="Q14" s="36">
-        <f t="shared" ref="Q14:Q18" si="14">B14-(G14+L14)</f>
+      <c r="Q14" s="70">
+        <f t="shared" ref="Q14:Q18" si="10">B14-(G14+L14)</f>
         <v>1.1166666666666671</v>
       </c>
-      <c r="R14" s="36">
+      <c r="R14" s="70">
         <f t="shared" si="6"/>
         <v>2.3333333333329875E-2</v>
       </c>
-      <c r="S14" s="36">
+      <c r="S14" s="70">
         <f t="shared" si="7"/>
         <v>0.63499999999999801</v>
       </c>
-      <c r="T14" s="36">
+      <c r="T14" s="70">
         <f t="shared" si="8"/>
         <v>-3.8633333333333439</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V14" s="1">
+        <f>_xlfn.VAR.S(L3:O3)</f>
+        <v>4.7949025462963064</v>
+      </c>
+    </row>
+    <row r="15" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B15" s="18">
         <v>26.88</v>
       </c>
@@ -3269,64 +3737,80 @@
         <v>32.74</v>
       </c>
       <c r="F15" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="G15" s="45">
+        <v>59</v>
+      </c>
+      <c r="G15" s="44">
         <f t="shared" si="9"/>
         <v>22.764583333333331</v>
       </c>
-      <c r="H15" s="39">
+      <c r="H15" s="38">
         <f t="shared" si="4"/>
         <v>22.764583333333331</v>
       </c>
-      <c r="I15" s="39">
+      <c r="I15" s="38">
         <f t="shared" si="4"/>
         <v>22.764583333333331</v>
       </c>
-      <c r="J15" s="44">
+      <c r="J15" s="43">
         <f t="shared" si="4"/>
         <v>22.764583333333331</v>
       </c>
       <c r="K15" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="L15" s="51">
+        <v>60</v>
+      </c>
+      <c r="L15" s="95">
+        <f t="shared" si="5"/>
+        <v>0.32875000000000298</v>
+      </c>
+      <c r="M15" s="95">
+        <f t="shared" si="5"/>
+        <v>-2.7879166666666606</v>
+      </c>
+      <c r="N15" s="95">
+        <f t="shared" si="5"/>
+        <v>-8.9583333333330017E-2</v>
+      </c>
+      <c r="O15" s="95">
+        <f t="shared" si="5"/>
+        <v>2.5487500000000125</v>
+      </c>
+      <c r="P15" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q15" s="70">
         <f t="shared" si="10"/>
-        <v>0.32875000000000298</v>
-      </c>
-      <c r="M15" s="51">
-        <f t="shared" si="11"/>
-        <v>-2.7879166666666606</v>
-      </c>
-      <c r="N15" s="51">
-        <f t="shared" si="12"/>
-        <v>-8.9583333333330017E-2</v>
-      </c>
-      <c r="O15" s="51">
-        <f t="shared" si="13"/>
-        <v>2.5487500000000125</v>
-      </c>
-      <c r="P15" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q15" s="36">
-        <f t="shared" si="14"/>
         <v>3.7866666666666653</v>
       </c>
-      <c r="R15" s="36">
+      <c r="R15" s="70">
         <f t="shared" si="6"/>
         <v>-0.10666666666666913</v>
       </c>
-      <c r="S15" s="36">
+      <c r="S15" s="70">
         <f t="shared" si="7"/>
         <v>-3.6850000000000023</v>
       </c>
-      <c r="T15" s="36">
+      <c r="T15" s="70">
         <f t="shared" si="8"/>
         <v>7.4266666666666588</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V15" s="1">
+        <f>_xlfn.VAR.S(Q13:Q18)</f>
+        <v>6.7526266666666626</v>
+      </c>
+      <c r="W15" s="1">
+        <f>_xlfn.VAR.S(R13:R18)</f>
+        <v>3.0156266666666656</v>
+      </c>
+      <c r="X15" s="1">
+        <f>_xlfn.VAR.S(S13:S18)</f>
+        <v>5.1711900000000011</v>
+      </c>
+      <c r="Y15" s="1">
+        <f>_xlfn.VAR.S(T13:T18)</f>
+        <v>15.172506666666672</v>
+      </c>
+    </row>
+    <row r="16" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B16" s="18">
         <v>21.6</v>
       </c>
@@ -3339,53 +3823,53 @@
       <c r="E16" s="18">
         <v>24.21</v>
       </c>
-      <c r="G16" s="45">
+      <c r="G16" s="44">
         <f t="shared" si="9"/>
         <v>22.764583333333331</v>
       </c>
-      <c r="H16" s="39">
+      <c r="H16" s="38">
         <f t="shared" si="4"/>
         <v>22.764583333333331</v>
       </c>
-      <c r="I16" s="39">
+      <c r="I16" s="38">
         <f t="shared" si="4"/>
         <v>22.764583333333331</v>
       </c>
-      <c r="J16" s="44">
+      <c r="J16" s="43">
         <f t="shared" si="4"/>
         <v>22.764583333333331</v>
       </c>
       <c r="K16" s="18"/>
-      <c r="L16" s="51">
+      <c r="L16" s="95">
+        <f t="shared" si="5"/>
+        <v>0.32875000000000298</v>
+      </c>
+      <c r="M16" s="95">
+        <f t="shared" si="5"/>
+        <v>-2.7879166666666606</v>
+      </c>
+      <c r="N16" s="95">
+        <f t="shared" si="5"/>
+        <v>-8.9583333333330017E-2</v>
+      </c>
+      <c r="O16" s="95">
+        <f t="shared" si="5"/>
+        <v>2.5487500000000125</v>
+      </c>
+      <c r="P16" s="18"/>
+      <c r="Q16" s="70">
         <f t="shared" si="10"/>
-        <v>0.32875000000000298</v>
-      </c>
-      <c r="M16" s="51">
-        <f t="shared" si="11"/>
-        <v>-2.7879166666666606</v>
-      </c>
-      <c r="N16" s="51">
-        <f t="shared" si="12"/>
-        <v>-8.9583333333330017E-2</v>
-      </c>
-      <c r="O16" s="51">
-        <f t="shared" si="13"/>
-        <v>2.5487500000000125</v>
-      </c>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="36">
-        <f t="shared" si="14"/>
         <v>-1.4933333333333323</v>
       </c>
-      <c r="R16" s="36">
+      <c r="R16" s="70">
         <f t="shared" si="6"/>
         <v>2.1133333333333297</v>
       </c>
-      <c r="S16" s="36">
+      <c r="S16" s="70">
         <f t="shared" si="7"/>
         <v>0.41499999999999915</v>
       </c>
-      <c r="T16" s="36">
+      <c r="T16" s="70">
         <f t="shared" si="8"/>
         <v>-1.1033333333333424</v>
       </c>
@@ -3403,53 +3887,53 @@
       <c r="E17" s="18">
         <v>25.67</v>
       </c>
-      <c r="G17" s="45">
+      <c r="G17" s="44">
         <f t="shared" si="9"/>
         <v>22.764583333333331</v>
       </c>
-      <c r="H17" s="39">
+      <c r="H17" s="38">
         <f t="shared" si="4"/>
         <v>22.764583333333331</v>
       </c>
-      <c r="I17" s="39">
+      <c r="I17" s="38">
         <f t="shared" si="4"/>
         <v>22.764583333333331</v>
       </c>
-      <c r="J17" s="44">
+      <c r="J17" s="43">
         <f t="shared" si="4"/>
         <v>22.764583333333331</v>
       </c>
       <c r="K17" s="18"/>
-      <c r="L17" s="51">
+      <c r="L17" s="95">
+        <f t="shared" si="5"/>
+        <v>0.32875000000000298</v>
+      </c>
+      <c r="M17" s="95">
+        <f t="shared" si="5"/>
+        <v>-2.7879166666666606</v>
+      </c>
+      <c r="N17" s="95">
+        <f t="shared" si="5"/>
+        <v>-8.9583333333330017E-2</v>
+      </c>
+      <c r="O17" s="95">
+        <f t="shared" si="5"/>
+        <v>2.5487500000000125</v>
+      </c>
+      <c r="P17" s="18"/>
+      <c r="Q17" s="70">
         <f t="shared" si="10"/>
-        <v>0.32875000000000298</v>
-      </c>
-      <c r="M17" s="51">
-        <f t="shared" si="11"/>
-        <v>-2.7879166666666606</v>
-      </c>
-      <c r="N17" s="51">
-        <f t="shared" si="12"/>
-        <v>-8.9583333333330017E-2</v>
-      </c>
-      <c r="O17" s="51">
-        <f t="shared" si="13"/>
-        <v>2.5487500000000125</v>
-      </c>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="36">
-        <f t="shared" si="14"/>
         <v>0.30666666666666487</v>
       </c>
-      <c r="R17" s="36">
+      <c r="R17" s="70">
         <f t="shared" si="6"/>
         <v>-2.3566666666666691</v>
       </c>
-      <c r="S17" s="36">
+      <c r="S17" s="70">
         <f t="shared" si="7"/>
         <v>1.134999999999998</v>
       </c>
-      <c r="T17" s="36">
+      <c r="T17" s="70">
         <f t="shared" si="8"/>
         <v>0.35666666666665847</v>
       </c>
@@ -3467,53 +3951,53 @@
       <c r="E18" s="18">
         <v>23.42</v>
       </c>
-      <c r="G18" s="46">
+      <c r="G18" s="45">
         <f t="shared" si="9"/>
         <v>22.764583333333331</v>
       </c>
-      <c r="H18" s="47">
+      <c r="H18" s="46">
         <f t="shared" si="4"/>
         <v>22.764583333333331</v>
       </c>
-      <c r="I18" s="47">
+      <c r="I18" s="46">
         <f t="shared" si="4"/>
         <v>22.764583333333331</v>
       </c>
-      <c r="J18" s="48">
+      <c r="J18" s="47">
         <f t="shared" si="4"/>
         <v>22.764583333333331</v>
       </c>
       <c r="K18" s="18"/>
-      <c r="L18" s="52">
+      <c r="L18" s="96">
+        <f t="shared" si="5"/>
+        <v>0.32875000000000298</v>
+      </c>
+      <c r="M18" s="96">
+        <f t="shared" si="5"/>
+        <v>-2.7879166666666606</v>
+      </c>
+      <c r="N18" s="96">
+        <f t="shared" si="5"/>
+        <v>-8.9583333333330017E-2</v>
+      </c>
+      <c r="O18" s="96">
+        <f t="shared" si="5"/>
+        <v>2.5487500000000125</v>
+      </c>
+      <c r="P18" s="18"/>
+      <c r="Q18" s="70">
         <f t="shared" si="10"/>
-        <v>0.32875000000000298</v>
-      </c>
-      <c r="M18" s="52">
-        <f t="shared" si="11"/>
-        <v>-2.7879166666666606</v>
-      </c>
-      <c r="N18" s="52">
-        <f t="shared" si="12"/>
-        <v>-8.9583333333330017E-2</v>
-      </c>
-      <c r="O18" s="52">
-        <f t="shared" si="13"/>
-        <v>2.5487500000000125</v>
-      </c>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="36">
-        <f t="shared" si="14"/>
         <v>0.25666666666666771</v>
       </c>
-      <c r="R18" s="36">
+      <c r="R18" s="70">
         <f t="shared" si="6"/>
         <v>1.7433333333333287</v>
       </c>
-      <c r="S18" s="36">
+      <c r="S18" s="70">
         <f t="shared" si="7"/>
         <v>-1.4050000000000011</v>
       </c>
-      <c r="T18" s="36">
+      <c r="T18" s="70">
         <f t="shared" si="8"/>
         <v>-1.8933333333333415</v>
       </c>
@@ -3522,12 +4006,12 @@
       <c r="C23" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="L23" s="57" t="s">
-        <v>63</v>
-      </c>
-      <c r="M23" s="57"/>
-      <c r="N23" s="57"/>
-      <c r="O23" s="57"/>
+      <c r="L23" s="98" t="s">
+        <v>61</v>
+      </c>
+      <c r="M23" s="98"/>
+      <c r="N23" s="98"/>
+      <c r="O23" s="98"/>
     </row>
     <row r="24" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B24" s="18" t="s">
@@ -3542,12 +4026,12 @@
       <c r="E24" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G24" s="58" t="s">
+      <c r="G24" s="100" t="s">
         <v>47</v>
       </c>
-      <c r="H24" s="58"/>
-      <c r="I24" s="58"/>
-      <c r="J24" s="58"/>
+      <c r="H24" s="100"/>
+      <c r="I24" s="100"/>
+      <c r="J24" s="100"/>
       <c r="L24" s="18" t="s">
         <v>4</v>
       </c>
@@ -3560,14 +4044,14 @@
       <c r="O24" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="Q24" s="59" t="s">
+      <c r="Q24" s="114" t="s">
         <v>48</v>
       </c>
-      <c r="R24" s="59"/>
-      <c r="S24" s="59"/>
-      <c r="T24" s="59"/>
-    </row>
-    <row r="25" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R24" s="114"/>
+      <c r="S24" s="114"/>
+      <c r="T24" s="114"/>
+    </row>
+    <row r="25" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <v>19.12</v>
       </c>
@@ -3580,21 +4064,21 @@
       <c r="E25" s="1">
         <v>24.39</v>
       </c>
-      <c r="G25" s="40"/>
-      <c r="H25" s="41"/>
-      <c r="I25" s="41"/>
-      <c r="J25" s="42"/>
-      <c r="L25" s="49"/>
-      <c r="M25" s="49"/>
-      <c r="N25" s="49"/>
-      <c r="O25" s="49"/>
-      <c r="Q25" s="37"/>
-      <c r="R25" s="37"/>
-      <c r="S25" s="37"/>
-      <c r="T25" s="37"/>
-    </row>
-    <row r="26" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="30">
+      <c r="G25" s="39"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="41"/>
+      <c r="L25" s="48"/>
+      <c r="M25" s="48"/>
+      <c r="N25" s="48"/>
+      <c r="O25" s="48"/>
+      <c r="Q25" s="36"/>
+      <c r="R25" s="36"/>
+      <c r="S25" s="36"/>
+      <c r="T25" s="36"/>
+    </row>
+    <row r="26" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B26" s="69">
         <v>24.21</v>
       </c>
       <c r="C26" s="1">
@@ -3606,26 +4090,20 @@
       <c r="E26" s="1">
         <v>21.45</v>
       </c>
-      <c r="G26" s="43">
-        <v>22.764583333333331</v>
-      </c>
-      <c r="H26" s="39"/>
-      <c r="I26" s="39"/>
-      <c r="J26" s="44"/>
-      <c r="L26" s="50">
-        <v>0.32875000000000298</v>
-      </c>
-      <c r="M26" s="51"/>
-      <c r="N26" s="51"/>
-      <c r="O26" s="51"/>
-      <c r="Q26" s="38">
-        <v>1.1166666666666671</v>
-      </c>
-      <c r="R26" s="37"/>
-      <c r="S26" s="37"/>
-      <c r="T26" s="37"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
+      <c r="J26" s="43"/>
+      <c r="L26" s="49"/>
+      <c r="M26" s="50"/>
+      <c r="N26" s="50"/>
+      <c r="O26" s="50"/>
+      <c r="Q26" s="37"/>
+      <c r="R26" s="36"/>
+      <c r="S26" s="36"/>
+      <c r="T26" s="36"/>
       <c r="Y26" s="33" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="2:25" x14ac:dyDescent="0.25">
@@ -3642,28 +4120,28 @@
         <v>32.74</v>
       </c>
       <c r="F27" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="G27" s="45"/>
-      <c r="H27" s="39"/>
-      <c r="I27" s="39"/>
-      <c r="J27" s="44"/>
+        <v>59</v>
+      </c>
+      <c r="G27" s="44"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="43"/>
       <c r="K27" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="L27" s="51"/>
-      <c r="M27" s="51"/>
-      <c r="N27" s="51"/>
-      <c r="O27" s="51"/>
+        <v>60</v>
+      </c>
+      <c r="L27" s="50"/>
+      <c r="M27" s="50"/>
+      <c r="N27" s="50"/>
+      <c r="O27" s="50"/>
       <c r="P27" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q27" s="37"/>
-      <c r="R27" s="37"/>
-      <c r="S27" s="37"/>
-      <c r="T27" s="37"/>
-    </row>
-    <row r="28" spans="2:25" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="Q27" s="36"/>
+      <c r="R27" s="36"/>
+      <c r="S27" s="36"/>
+      <c r="T27" s="36"/>
+    </row>
+    <row r="28" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="1">
         <v>21.6</v>
       </c>
@@ -3676,24 +4154,24 @@
       <c r="E28" s="1">
         <v>24.21</v>
       </c>
-      <c r="G28" s="45"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="44"/>
-      <c r="L28" s="51"/>
-      <c r="M28" s="51"/>
-      <c r="N28" s="51"/>
-      <c r="O28" s="51"/>
-      <c r="Q28" s="37"/>
-      <c r="R28" s="37"/>
-      <c r="S28" s="37"/>
-      <c r="T28" s="37"/>
-    </row>
-    <row r="29" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="G28" s="44"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="43"/>
+      <c r="L28" s="50"/>
+      <c r="M28" s="50"/>
+      <c r="N28" s="50"/>
+      <c r="O28" s="50"/>
+      <c r="Q28" s="36"/>
+      <c r="R28" s="36"/>
+      <c r="S28" s="36"/>
+      <c r="T28" s="36"/>
+    </row>
+    <row r="29" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="1">
         <v>23.4</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="30">
         <v>17.62</v>
       </c>
       <c r="D29" s="1">
@@ -3702,18 +4180,27 @@
       <c r="E29" s="1">
         <v>25.67</v>
       </c>
-      <c r="G29" s="45"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="44"/>
-      <c r="L29" s="51"/>
-      <c r="M29" s="51"/>
-      <c r="N29" s="51"/>
-      <c r="O29" s="51"/>
-      <c r="Q29" s="37"/>
-      <c r="R29" s="37"/>
-      <c r="S29" s="37"/>
-      <c r="T29" s="37"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="72">
+        <f>H17</f>
+        <v>22.764583333333331</v>
+      </c>
+      <c r="I29" s="38"/>
+      <c r="J29" s="43"/>
+      <c r="L29" s="50"/>
+      <c r="M29" s="71">
+        <f>M17</f>
+        <v>-2.7879166666666606</v>
+      </c>
+      <c r="N29" s="50"/>
+      <c r="O29" s="50"/>
+      <c r="Q29" s="36"/>
+      <c r="R29" s="73">
+        <f>R17</f>
+        <v>-2.3566666666666691</v>
+      </c>
+      <c r="S29" s="36"/>
+      <c r="T29" s="36"/>
     </row>
     <row r="30" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
@@ -3728,31 +4215,34 @@
       <c r="E30" s="1">
         <v>23.42</v>
       </c>
-      <c r="G30" s="46"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="48"/>
-      <c r="L30" s="52"/>
-      <c r="M30" s="52"/>
-      <c r="N30" s="52"/>
-      <c r="O30" s="52"/>
-      <c r="Q30" s="37"/>
-      <c r="R30" s="37"/>
-      <c r="S30" s="37"/>
-      <c r="T30" s="37"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="46"/>
+      <c r="I30" s="46"/>
+      <c r="J30" s="47"/>
+      <c r="L30" s="51"/>
+      <c r="M30" s="51"/>
+      <c r="N30" s="51"/>
+      <c r="O30" s="51"/>
+      <c r="Q30" s="36"/>
+      <c r="R30" s="36"/>
+      <c r="S30" s="36"/>
+      <c r="T30" s="36"/>
+    </row>
+    <row r="32" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="H32" s="74"/>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C33" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="L33" s="57" t="s">
-        <v>63</v>
-      </c>
-      <c r="M33" s="57"/>
-      <c r="N33" s="57"/>
-      <c r="O33" s="57"/>
-    </row>
-    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="L33" s="98" t="s">
+        <v>61</v>
+      </c>
+      <c r="M33" s="98"/>
+      <c r="N33" s="98"/>
+      <c r="O33" s="98"/>
+    </row>
+    <row r="34" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="18" t="s">
         <v>4</v>
       </c>
@@ -3765,12 +4255,12 @@
       <c r="E34" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G34" s="60" t="s">
+      <c r="G34" s="101" t="s">
         <v>47</v>
       </c>
-      <c r="H34" s="60"/>
-      <c r="I34" s="60"/>
-      <c r="J34" s="60"/>
+      <c r="H34" s="101"/>
+      <c r="I34" s="101"/>
+      <c r="J34" s="101"/>
       <c r="L34" s="18" t="s">
         <v>4</v>
       </c>
@@ -3783,239 +4273,648 @@
       <c r="O34" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q34" s="59" t="s">
+      <c r="Q34" s="114" t="s">
         <v>48</v>
       </c>
-      <c r="R34" s="59"/>
-      <c r="S34" s="59"/>
-      <c r="T34" s="59"/>
+      <c r="R34" s="114"/>
+      <c r="S34" s="114"/>
+      <c r="T34" s="114"/>
     </row>
     <row r="35" spans="2:20" ht="20.25" x14ac:dyDescent="0.35">
       <c r="B35" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="D35" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="C35" s="32" t="s">
+      <c r="E35" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="D35" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="E35" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="G35" s="61" t="s">
+      <c r="G35" s="102" t="s">
+        <v>86</v>
+      </c>
+      <c r="H35" s="103"/>
+      <c r="I35" s="103"/>
+      <c r="J35" s="104"/>
+      <c r="L35" s="111" t="s">
+        <v>87</v>
+      </c>
+      <c r="M35" s="111" t="s">
         <v>88</v>
       </c>
-      <c r="H35" s="62"/>
-      <c r="I35" s="62"/>
-      <c r="J35" s="63"/>
-      <c r="L35" s="70" t="s">
+      <c r="N35" s="111" t="s">
         <v>89</v>
       </c>
-      <c r="M35" s="70" t="s">
+      <c r="O35" s="111" t="s">
         <v>90</v>
       </c>
-      <c r="N35" s="70" t="s">
+      <c r="Q35" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="O35" s="70" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q35" s="32" t="s">
-        <v>93</v>
-      </c>
       <c r="R35" s="32" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="S35" s="32" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="T35" s="32" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="2:20" ht="20.25" x14ac:dyDescent="0.35">
       <c r="B36" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="D36" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="C36" s="32" t="s">
+      <c r="E36" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="D36" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="E36" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="G36" s="64"/>
-      <c r="H36" s="65"/>
-      <c r="I36" s="65"/>
-      <c r="J36" s="66"/>
-      <c r="L36" s="71"/>
-      <c r="M36" s="71"/>
-      <c r="N36" s="71"/>
-      <c r="O36" s="71"/>
+      <c r="G36" s="105"/>
+      <c r="H36" s="106"/>
+      <c r="I36" s="106"/>
+      <c r="J36" s="107"/>
+      <c r="L36" s="112"/>
+      <c r="M36" s="112"/>
+      <c r="N36" s="112"/>
+      <c r="O36" s="112"/>
       <c r="Q36" s="32" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="R36" s="32" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="S36" s="32" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="T36" s="32" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="2:20" ht="20.25" x14ac:dyDescent="0.35">
       <c r="B37" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="D37" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="C37" s="32" t="s">
+      <c r="E37" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="D37" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="E37" s="32" t="s">
-        <v>75</v>
-      </c>
       <c r="F37" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="G37" s="64"/>
-      <c r="H37" s="65"/>
-      <c r="I37" s="65"/>
-      <c r="J37" s="66"/>
+        <v>59</v>
+      </c>
+      <c r="G37" s="105"/>
+      <c r="H37" s="106"/>
+      <c r="I37" s="106"/>
+      <c r="J37" s="107"/>
       <c r="K37" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="L37" s="71"/>
-      <c r="M37" s="71"/>
-      <c r="N37" s="71"/>
-      <c r="O37" s="71"/>
+        <v>60</v>
+      </c>
+      <c r="L37" s="112"/>
+      <c r="M37" s="112"/>
+      <c r="N37" s="112"/>
+      <c r="O37" s="112"/>
       <c r="P37" s="29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="Q37" s="32" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="R37" s="32" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="S37" s="32" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="T37" s="32" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="2:20" ht="20.25" x14ac:dyDescent="0.35">
       <c r="B38" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="C38" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="D38" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="C38" s="32" t="s">
+      <c r="E38" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="D38" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="E38" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="G38" s="64"/>
-      <c r="H38" s="65"/>
-      <c r="I38" s="65"/>
-      <c r="J38" s="66"/>
-      <c r="L38" s="71"/>
-      <c r="M38" s="71"/>
-      <c r="N38" s="71"/>
-      <c r="O38" s="71"/>
+      <c r="G38" s="105"/>
+      <c r="H38" s="106"/>
+      <c r="I38" s="106"/>
+      <c r="J38" s="107"/>
+      <c r="L38" s="112"/>
+      <c r="M38" s="112"/>
+      <c r="N38" s="112"/>
+      <c r="O38" s="112"/>
       <c r="Q38" s="32" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="R38" s="32" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="S38" s="32" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="T38" s="32" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" spans="2:20" ht="20.25" x14ac:dyDescent="0.35">
       <c r="B39" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="D39" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="C39" s="32" t="s">
+      <c r="E39" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="D39" s="32" t="s">
+      <c r="G39" s="105"/>
+      <c r="H39" s="106"/>
+      <c r="I39" s="106"/>
+      <c r="J39" s="107"/>
+      <c r="L39" s="112"/>
+      <c r="M39" s="112"/>
+      <c r="N39" s="112"/>
+      <c r="O39" s="112"/>
+      <c r="Q39" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="R39" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="S39" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="T39" s="32" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="2:20" ht="21" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B40" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="E39" s="32" t="s">
+      <c r="C40" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="G39" s="64"/>
-      <c r="H39" s="65"/>
-      <c r="I39" s="65"/>
-      <c r="J39" s="66"/>
-      <c r="L39" s="71"/>
-      <c r="M39" s="71"/>
-      <c r="N39" s="71"/>
-      <c r="O39" s="71"/>
-      <c r="Q39" s="32" t="s">
-        <v>98</v>
-      </c>
-      <c r="R39" s="32" t="s">
-        <v>104</v>
-      </c>
-      <c r="S39" s="32" t="s">
-        <v>110</v>
-      </c>
-      <c r="T39" s="32" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="40" spans="2:20" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="B40" s="32" t="s">
+      <c r="D40" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="C40" s="32" t="s">
+      <c r="E40" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="D40" s="32" t="s">
+      <c r="G40" s="108"/>
+      <c r="H40" s="109"/>
+      <c r="I40" s="109"/>
+      <c r="J40" s="110"/>
+      <c r="L40" s="113"/>
+      <c r="M40" s="113"/>
+      <c r="N40" s="113"/>
+      <c r="O40" s="113"/>
+      <c r="Q40" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="R40" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="S40" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="T40" s="32" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="44" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C44" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="L44" s="98" t="s">
+        <v>61</v>
+      </c>
+      <c r="M44" s="98"/>
+      <c r="N44" s="98"/>
+      <c r="O44" s="98"/>
+    </row>
+    <row r="45" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E45" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G45" s="101" t="s">
+        <v>47</v>
+      </c>
+      <c r="H45" s="101"/>
+      <c r="I45" s="101"/>
+      <c r="J45" s="101"/>
+      <c r="L45" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N45" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q45" s="100" t="s">
+        <v>48</v>
+      </c>
+      <c r="R45" s="100"/>
+      <c r="S45" s="100"/>
+      <c r="T45" s="100"/>
+    </row>
+    <row r="46" spans="2:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B46" s="76"/>
+      <c r="C46" s="76"/>
+      <c r="D46" s="76"/>
+      <c r="E46" s="76"/>
+      <c r="G46" s="102"/>
+      <c r="H46" s="103"/>
+      <c r="I46" s="103"/>
+      <c r="J46" s="104"/>
+      <c r="L46" s="111"/>
+      <c r="M46" s="111"/>
+      <c r="N46" s="111"/>
+      <c r="O46" s="111"/>
+      <c r="Q46" s="76"/>
+      <c r="R46" s="76"/>
+      <c r="S46" s="76"/>
+      <c r="T46" s="76"/>
+    </row>
+    <row r="47" spans="2:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B47" s="76"/>
+      <c r="C47" s="76"/>
+      <c r="D47" s="76"/>
+      <c r="E47" s="76"/>
+      <c r="G47" s="105"/>
+      <c r="H47" s="106"/>
+      <c r="I47" s="106"/>
+      <c r="J47" s="107"/>
+      <c r="L47" s="112"/>
+      <c r="M47" s="112"/>
+      <c r="N47" s="112"/>
+      <c r="O47" s="112"/>
+      <c r="Q47" s="76"/>
+      <c r="R47" s="76"/>
+      <c r="S47" s="76"/>
+      <c r="T47" s="76"/>
+    </row>
+    <row r="48" spans="2:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="76"/>
+      <c r="C48" s="76"/>
+      <c r="D48" s="76"/>
+      <c r="E48" s="76"/>
+      <c r="F48" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="G48" s="105"/>
+      <c r="H48" s="106"/>
+      <c r="I48" s="106"/>
+      <c r="J48" s="107"/>
+      <c r="K48" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="L48" s="112"/>
+      <c r="M48" s="112"/>
+      <c r="N48" s="112"/>
+      <c r="O48" s="112"/>
+      <c r="P48" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q48" s="76"/>
+      <c r="R48" s="76"/>
+      <c r="S48" s="76"/>
+      <c r="T48" s="76"/>
+    </row>
+    <row r="49" spans="1:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B49" s="76"/>
+      <c r="C49" s="76"/>
+      <c r="D49" s="76"/>
+      <c r="E49" s="76"/>
+      <c r="G49" s="105"/>
+      <c r="H49" s="106"/>
+      <c r="I49" s="106"/>
+      <c r="J49" s="107"/>
+      <c r="L49" s="112"/>
+      <c r="M49" s="112"/>
+      <c r="N49" s="112"/>
+      <c r="O49" s="112"/>
+      <c r="Q49" s="76"/>
+      <c r="R49" s="76"/>
+      <c r="S49" s="76"/>
+      <c r="T49" s="76"/>
+    </row>
+    <row r="50" spans="1:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="76"/>
+      <c r="C50" s="76"/>
+      <c r="D50" s="76"/>
+      <c r="E50" s="76"/>
+      <c r="G50" s="105"/>
+      <c r="H50" s="106"/>
+      <c r="I50" s="106"/>
+      <c r="J50" s="107"/>
+      <c r="L50" s="112"/>
+      <c r="M50" s="112"/>
+      <c r="N50" s="112"/>
+      <c r="O50" s="112"/>
+      <c r="Q50" s="76"/>
+      <c r="R50" s="76"/>
+      <c r="S50" s="76"/>
+      <c r="T50" s="76"/>
+    </row>
+    <row r="51" spans="1:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B51" s="76"/>
+      <c r="C51" s="76"/>
+      <c r="D51" s="76"/>
+      <c r="E51" s="76"/>
+      <c r="G51" s="108"/>
+      <c r="H51" s="109"/>
+      <c r="I51" s="109"/>
+      <c r="J51" s="110"/>
+      <c r="L51" s="113"/>
+      <c r="M51" s="113"/>
+      <c r="N51" s="113"/>
+      <c r="O51" s="113"/>
+      <c r="Q51" s="76"/>
+      <c r="R51" s="76"/>
+      <c r="S51" s="76"/>
+      <c r="T51" s="76"/>
+    </row>
+    <row r="53" spans="1:20" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="B53" s="99" t="s">
+        <v>121</v>
+      </c>
+      <c r="C53" s="99"/>
+      <c r="D53" s="99"/>
+      <c r="E53" s="99"/>
+      <c r="F53" s="77" t="s">
+        <v>59</v>
+      </c>
+      <c r="G53" s="99" t="s">
         <v>86</v>
       </c>
-      <c r="E40" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="G40" s="67"/>
-      <c r="H40" s="68"/>
-      <c r="I40" s="68"/>
-      <c r="J40" s="69"/>
-      <c r="L40" s="72"/>
-      <c r="M40" s="72"/>
-      <c r="N40" s="72"/>
-      <c r="O40" s="72"/>
-      <c r="Q40" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="R40" s="32" t="s">
-        <v>105</v>
-      </c>
-      <c r="S40" s="32" t="s">
-        <v>111</v>
-      </c>
-      <c r="T40" s="32" t="s">
-        <v>117</v>
-      </c>
+      <c r="H53" s="99"/>
+      <c r="I53" s="99"/>
+      <c r="J53" s="99"/>
+      <c r="K53" s="77" t="s">
+        <v>60</v>
+      </c>
+      <c r="L53" s="99" t="s">
+        <v>122</v>
+      </c>
+      <c r="M53" s="99"/>
+      <c r="N53" s="99"/>
+      <c r="O53" s="99"/>
+      <c r="P53" s="77" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q53" s="99" t="s">
+        <v>123</v>
+      </c>
+      <c r="R53" s="99"/>
+      <c r="S53" s="99"/>
+      <c r="T53" s="99"/>
+    </row>
+    <row r="59" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="68"/>
+      <c r="C59" s="120" t="s">
+        <v>58</v>
+      </c>
+      <c r="D59" s="68"/>
+      <c r="E59" s="68"/>
+      <c r="G59" s="123" t="s">
+        <v>47</v>
+      </c>
+      <c r="H59" s="123"/>
+      <c r="I59" s="123"/>
+      <c r="J59" s="123"/>
+      <c r="L59" s="98" t="s">
+        <v>143</v>
+      </c>
+      <c r="M59" s="98"/>
+      <c r="N59" s="98"/>
+      <c r="O59" s="98"/>
+      <c r="Q59" s="100" t="s">
+        <v>48</v>
+      </c>
+      <c r="R59" s="100"/>
+      <c r="S59" s="100"/>
+      <c r="T59" s="100"/>
+    </row>
+    <row r="60" spans="1:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="57"/>
+      <c r="B60" s="76"/>
+      <c r="C60" s="76"/>
+      <c r="D60" s="76"/>
+      <c r="E60" s="76"/>
+      <c r="F60" s="63"/>
+      <c r="G60" s="121"/>
+      <c r="H60" s="122"/>
+      <c r="I60" s="122"/>
+      <c r="J60" s="122"/>
+      <c r="K60" s="63"/>
+      <c r="L60" s="111"/>
+      <c r="M60" s="111"/>
+      <c r="N60" s="111"/>
+      <c r="O60" s="111"/>
+      <c r="Q60" s="76"/>
+      <c r="R60" s="76"/>
+      <c r="S60" s="76"/>
+      <c r="T60" s="76"/>
+    </row>
+    <row r="61" spans="1:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="57"/>
+      <c r="B61" s="76"/>
+      <c r="C61" s="76"/>
+      <c r="D61" s="76"/>
+      <c r="E61" s="76"/>
+      <c r="F61" s="63"/>
+      <c r="G61" s="122"/>
+      <c r="H61" s="122"/>
+      <c r="I61" s="122"/>
+      <c r="J61" s="122"/>
+      <c r="K61" s="63"/>
+      <c r="L61" s="112"/>
+      <c r="M61" s="112"/>
+      <c r="N61" s="112"/>
+      <c r="O61" s="112"/>
+      <c r="Q61" s="76"/>
+      <c r="R61" s="76"/>
+      <c r="S61" s="76"/>
+      <c r="T61" s="76"/>
+    </row>
+    <row r="62" spans="1:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="57"/>
+      <c r="B62" s="76"/>
+      <c r="C62" s="76"/>
+      <c r="D62" s="76"/>
+      <c r="E62" s="76"/>
+      <c r="F62" s="124" t="s">
+        <v>59</v>
+      </c>
+      <c r="G62" s="122"/>
+      <c r="H62" s="122"/>
+      <c r="I62" s="122"/>
+      <c r="J62" s="122"/>
+      <c r="K62" s="124" t="s">
+        <v>60</v>
+      </c>
+      <c r="L62" s="112"/>
+      <c r="M62" s="112"/>
+      <c r="N62" s="112"/>
+      <c r="O62" s="112"/>
+      <c r="P62" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q62" s="76"/>
+      <c r="R62" s="76"/>
+      <c r="S62" s="76"/>
+      <c r="T62" s="76"/>
+    </row>
+    <row r="63" spans="1:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="57"/>
+      <c r="B63" s="76"/>
+      <c r="C63" s="76"/>
+      <c r="D63" s="76"/>
+      <c r="E63" s="76"/>
+      <c r="F63" s="63"/>
+      <c r="G63" s="122"/>
+      <c r="H63" s="122"/>
+      <c r="I63" s="122"/>
+      <c r="J63" s="122"/>
+      <c r="L63" s="112"/>
+      <c r="M63" s="112"/>
+      <c r="N63" s="112"/>
+      <c r="O63" s="112"/>
+      <c r="Q63" s="76"/>
+      <c r="R63" s="76"/>
+      <c r="S63" s="76"/>
+      <c r="T63" s="76"/>
+    </row>
+    <row r="64" spans="1:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="57"/>
+      <c r="B64" s="76"/>
+      <c r="C64" s="76"/>
+      <c r="D64" s="76"/>
+      <c r="E64" s="76"/>
+      <c r="F64" s="63"/>
+      <c r="G64" s="122"/>
+      <c r="H64" s="122"/>
+      <c r="I64" s="122"/>
+      <c r="J64" s="122"/>
+      <c r="L64" s="112"/>
+      <c r="M64" s="112"/>
+      <c r="N64" s="112"/>
+      <c r="O64" s="112"/>
+      <c r="Q64" s="76"/>
+      <c r="R64" s="76"/>
+      <c r="S64" s="76"/>
+      <c r="T64" s="76"/>
+    </row>
+    <row r="65" spans="1:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="57"/>
+      <c r="B65" s="76"/>
+      <c r="C65" s="76"/>
+      <c r="D65" s="76"/>
+      <c r="E65" s="76"/>
+      <c r="F65" s="63"/>
+      <c r="G65" s="122"/>
+      <c r="H65" s="122"/>
+      <c r="I65" s="122"/>
+      <c r="J65" s="122"/>
+      <c r="L65" s="113"/>
+      <c r="M65" s="113"/>
+      <c r="N65" s="113"/>
+      <c r="O65" s="113"/>
+      <c r="Q65" s="76"/>
+      <c r="R65" s="76"/>
+      <c r="S65" s="76"/>
+      <c r="T65" s="76"/>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="G66" s="83"/>
+      <c r="H66" s="83"/>
+      <c r="I66" s="83"/>
+      <c r="J66" s="83"/>
+    </row>
+    <row r="67" spans="1:20" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="B67" s="99" t="s">
+        <v>121</v>
+      </c>
+      <c r="C67" s="99"/>
+      <c r="D67" s="99"/>
+      <c r="E67" s="99"/>
+      <c r="F67" s="77" t="s">
+        <v>59</v>
+      </c>
+      <c r="G67" s="99" t="s">
+        <v>86</v>
+      </c>
+      <c r="H67" s="99"/>
+      <c r="I67" s="99"/>
+      <c r="J67" s="99"/>
+      <c r="K67" s="77" t="s">
+        <v>60</v>
+      </c>
+      <c r="L67" s="99" t="s">
+        <v>122</v>
+      </c>
+      <c r="M67" s="99"/>
+      <c r="N67" s="99"/>
+      <c r="O67" s="99"/>
+      <c r="P67" s="77" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q67" s="99" t="s">
+        <v>123</v>
+      </c>
+      <c r="R67" s="99"/>
+      <c r="S67" s="99"/>
+      <c r="T67" s="99"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="L33:O33"/>
+  <mergeCells count="40">
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="G67:J67"/>
+    <mergeCell ref="L67:O67"/>
+    <mergeCell ref="Q67:T67"/>
+    <mergeCell ref="L59:O59"/>
+    <mergeCell ref="G59:J59"/>
+    <mergeCell ref="Q59:T59"/>
+    <mergeCell ref="G60:J65"/>
+    <mergeCell ref="L60:L65"/>
+    <mergeCell ref="M60:M65"/>
+    <mergeCell ref="N60:N65"/>
+    <mergeCell ref="O60:O65"/>
     <mergeCell ref="G34:J34"/>
     <mergeCell ref="Q34:T34"/>
     <mergeCell ref="G35:J40"/>
@@ -4023,12 +4922,27 @@
     <mergeCell ref="M35:M40"/>
     <mergeCell ref="N35:N40"/>
     <mergeCell ref="O35:O40"/>
-    <mergeCell ref="L23:O23"/>
-    <mergeCell ref="G24:J24"/>
     <mergeCell ref="Q24:T24"/>
     <mergeCell ref="L11:O11"/>
     <mergeCell ref="G12:J12"/>
     <mergeCell ref="Q12:T12"/>
+    <mergeCell ref="L33:O33"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="B53:E53"/>
+    <mergeCell ref="G53:J53"/>
+    <mergeCell ref="L53:O53"/>
+    <mergeCell ref="Q53:T53"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="L44:O44"/>
+    <mergeCell ref="G45:J45"/>
+    <mergeCell ref="Q45:T45"/>
+    <mergeCell ref="G46:J51"/>
+    <mergeCell ref="L46:L51"/>
+    <mergeCell ref="M46:M51"/>
+    <mergeCell ref="N46:N51"/>
+    <mergeCell ref="O46:O51"/>
+    <mergeCell ref="L23:O23"/>
+    <mergeCell ref="G24:J24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4433,8 +5347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="C5:AY51"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="P40" sqref="P40"/>
+    <sheetView topLeftCell="P22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AB37" sqref="AB37:AE42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4574,7 +5488,7 @@
       <c r="S7" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="U7" s="74" t="s">
+      <c r="U7" s="116" t="s">
         <v>37</v>
       </c>
       <c r="V7" s="9" t="s">
@@ -4586,7 +5500,7 @@
       <c r="X7" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="Z7" s="74" t="s">
+      <c r="Z7" s="116" t="s">
         <v>37</v>
       </c>
       <c r="AA7" s="9" t="s">
@@ -4618,7 +5532,7 @@
       <c r="S8" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="U8" s="74"/>
+      <c r="U8" s="116"/>
       <c r="V8" s="15" t="s">
         <v>26</v>
       </c>
@@ -4628,7 +5542,7 @@
       <c r="X8" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="Z8" s="74"/>
+      <c r="Z8" s="116"/>
       <c r="AA8" s="15" t="s">
         <v>26</v>
       </c>
@@ -4658,7 +5572,7 @@
       <c r="S9" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="U9" s="75" t="s">
+      <c r="U9" s="117" t="s">
         <v>38</v>
       </c>
       <c r="V9" s="12" t="s">
@@ -4670,7 +5584,7 @@
       <c r="X9" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="Z9" s="75" t="s">
+      <c r="Z9" s="117" t="s">
         <v>38</v>
       </c>
       <c r="AA9" s="12" t="s">
@@ -4693,7 +5607,7 @@
       <c r="S10" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="U10" s="75"/>
+      <c r="U10" s="117"/>
       <c r="V10" s="15" t="s">
         <v>28</v>
       </c>
@@ -4703,7 +5617,7 @@
       <c r="X10" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="Z10" s="75"/>
+      <c r="Z10" s="117"/>
       <c r="AA10" s="15" t="s">
         <v>28</v>
       </c>
@@ -4819,24 +5733,24 @@
       </c>
     </row>
     <row r="26" spans="7:43" x14ac:dyDescent="0.25">
-      <c r="AB26" s="73" t="s">
-        <v>120</v>
-      </c>
-      <c r="AC26" s="73"/>
-      <c r="AD26" s="73"/>
-      <c r="AE26" s="73"/>
-      <c r="AH26" s="73" t="s">
+      <c r="AB26" s="115" t="s">
+        <v>118</v>
+      </c>
+      <c r="AC26" s="115"/>
+      <c r="AD26" s="115"/>
+      <c r="AE26" s="115"/>
+      <c r="AH26" s="115" t="s">
         <v>50</v>
       </c>
-      <c r="AI26" s="73"/>
-      <c r="AJ26" s="73"/>
-      <c r="AK26" s="73"/>
-      <c r="AN26" s="73" t="s">
-        <v>121</v>
-      </c>
-      <c r="AO26" s="73"/>
-      <c r="AP26" s="73"/>
-      <c r="AQ26" s="73"/>
+      <c r="AI26" s="115"/>
+      <c r="AJ26" s="115"/>
+      <c r="AK26" s="115"/>
+      <c r="AN26" s="115" t="s">
+        <v>119</v>
+      </c>
+      <c r="AO26" s="115"/>
+      <c r="AP26" s="115"/>
+      <c r="AQ26" s="115"/>
     </row>
     <row r="27" spans="7:43" x14ac:dyDescent="0.25">
       <c r="G27" t="s">
@@ -4863,22 +5777,22 @@
       <c r="P27" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="Q27" s="54">
+      <c r="Q27" s="53">
         <v>19.12</v>
       </c>
-      <c r="R27" s="55">
+      <c r="R27" s="54">
         <v>24.21</v>
       </c>
-      <c r="S27" s="55">
+      <c r="S27" s="54">
         <v>26.88</v>
       </c>
-      <c r="T27" s="55">
+      <c r="T27" s="54">
         <v>21.6</v>
       </c>
-      <c r="U27" s="55">
+      <c r="U27" s="54">
         <v>23.4</v>
       </c>
-      <c r="V27" s="56">
+      <c r="V27" s="55">
         <v>23.35</v>
       </c>
       <c r="AB27" s="18" t="s">
@@ -4935,22 +5849,22 @@
       <c r="P28" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="Q28" s="54">
+      <c r="Q28" s="53">
         <v>18.559999999999999</v>
       </c>
-      <c r="R28" s="55">
+      <c r="R28" s="54">
         <v>20</v>
       </c>
-      <c r="S28" s="55">
+      <c r="S28" s="54">
         <v>19.87</v>
       </c>
-      <c r="T28" s="55">
+      <c r="T28" s="54">
         <v>22.09</v>
       </c>
-      <c r="U28" s="55">
+      <c r="U28" s="54">
         <v>17.62</v>
       </c>
-      <c r="V28" s="56">
+      <c r="V28" s="55">
         <v>21.72</v>
       </c>
       <c r="AB28" s="9">
@@ -4965,8 +5879,8 @@
       <c r="AE28" s="11">
         <v>24.39</v>
       </c>
-      <c r="AG28" s="74" t="s">
-        <v>119</v>
+      <c r="AG28" s="116" t="s">
+        <v>117</v>
       </c>
       <c r="AH28" s="9">
         <v>19.12</v>
@@ -4980,8 +5894,8 @@
       <c r="AK28" s="11">
         <v>24.39</v>
       </c>
-      <c r="AM28" s="74" t="s">
-        <v>119</v>
+      <c r="AM28" s="116" t="s">
+        <v>117</v>
       </c>
       <c r="AN28" s="9">
         <v>19.12</v>
@@ -5021,22 +5935,22 @@
       <c r="P29" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="Q29" s="54">
+      <c r="Q29" s="53">
         <v>25.58</v>
       </c>
-      <c r="R29" s="55">
+      <c r="R29" s="54">
         <v>23.31</v>
       </c>
-      <c r="S29" s="55">
+      <c r="S29" s="54">
         <v>18.989999999999998</v>
       </c>
-      <c r="T29" s="55">
+      <c r="T29" s="54">
         <v>23.09</v>
       </c>
-      <c r="U29" s="55">
+      <c r="U29" s="54">
         <v>23.81</v>
       </c>
-      <c r="V29" s="56">
+      <c r="V29" s="55">
         <v>21.27</v>
       </c>
       <c r="AB29" s="12">
@@ -5051,7 +5965,7 @@
       <c r="AE29" s="14">
         <v>21.45</v>
       </c>
-      <c r="AG29" s="74"/>
+      <c r="AG29" s="116"/>
       <c r="AH29" s="12">
         <v>24.21</v>
       </c>
@@ -5064,7 +5978,7 @@
       <c r="AK29" s="14">
         <v>21.45</v>
       </c>
-      <c r="AM29" s="74"/>
+      <c r="AM29" s="116"/>
       <c r="AN29" s="12">
         <v>24.21</v>
       </c>
@@ -5103,22 +6017,22 @@
       <c r="P30" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="Q30" s="54">
+      <c r="Q30" s="53">
         <v>24.39</v>
       </c>
-      <c r="R30" s="55">
+      <c r="R30" s="54">
         <v>21.45</v>
       </c>
-      <c r="S30" s="55">
+      <c r="S30" s="54">
         <v>32.74</v>
       </c>
-      <c r="T30" s="55">
+      <c r="T30" s="54">
         <v>24.21</v>
       </c>
-      <c r="U30" s="55">
+      <c r="U30" s="54">
         <v>25.67</v>
       </c>
-      <c r="V30" s="56">
+      <c r="V30" s="55">
         <v>23.42</v>
       </c>
       <c r="AB30" s="12">
@@ -5133,7 +6047,7 @@
       <c r="AE30" s="14">
         <v>32.74</v>
       </c>
-      <c r="AG30" s="74"/>
+      <c r="AG30" s="116"/>
       <c r="AH30" s="12">
         <v>26.88</v>
       </c>
@@ -5146,7 +6060,7 @@
       <c r="AK30" s="14">
         <v>32.74</v>
       </c>
-      <c r="AM30" s="74"/>
+      <c r="AM30" s="116"/>
       <c r="AN30" s="15">
         <v>26.88</v>
       </c>
@@ -5194,8 +6108,8 @@
       <c r="AE31" s="14">
         <v>24.21</v>
       </c>
-      <c r="AG31" s="74" t="s">
-        <v>118</v>
+      <c r="AG31" s="116" t="s">
+        <v>116</v>
       </c>
       <c r="AH31" s="9">
         <v>21.6</v>
@@ -5209,8 +6123,8 @@
       <c r="AK31" s="11">
         <v>24.21</v>
       </c>
-      <c r="AM31" s="74" t="s">
-        <v>118</v>
+      <c r="AM31" s="116" t="s">
+        <v>116</v>
       </c>
       <c r="AN31" s="12">
         <v>21.6</v>
@@ -5259,7 +6173,7 @@
       <c r="AE32" s="14">
         <v>25.67</v>
       </c>
-      <c r="AG32" s="74"/>
+      <c r="AG32" s="116"/>
       <c r="AH32" s="12">
         <v>23.4</v>
       </c>
@@ -5272,7 +6186,7 @@
       <c r="AK32" s="14">
         <v>25.67</v>
       </c>
-      <c r="AM32" s="74"/>
+      <c r="AM32" s="116"/>
       <c r="AN32" s="12">
         <v>23.4</v>
       </c>
@@ -5320,7 +6234,7 @@
       <c r="AE33" s="17">
         <v>23.42</v>
       </c>
-      <c r="AG33" s="74"/>
+      <c r="AG33" s="116"/>
       <c r="AH33" s="15">
         <v>23.35</v>
       </c>
@@ -5333,7 +6247,7 @@
       <c r="AK33" s="17">
         <v>23.42</v>
       </c>
-      <c r="AM33" s="74"/>
+      <c r="AM33" s="116"/>
       <c r="AN33" s="15">
         <v>23.35</v>
       </c>
@@ -5430,7 +6344,7 @@
       <c r="I37">
         <v>22.09</v>
       </c>
-      <c r="K37" s="54">
+      <c r="K37" s="53">
         <v>23.09</v>
       </c>
       <c r="L37" s="23">
@@ -5439,7 +6353,7 @@
       <c r="M37" s="23">
         <v>22.68</v>
       </c>
-      <c r="N37" s="56">
+      <c r="N37" s="55">
         <v>25.31</v>
       </c>
       <c r="AB37" s="9">
@@ -5454,7 +6368,7 @@
       <c r="AE37" s="11">
         <v>24.39</v>
       </c>
-      <c r="AG37" s="74" t="s">
+      <c r="AG37" s="116" t="s">
         <v>42</v>
       </c>
       <c r="AH37" s="9">
@@ -5469,7 +6383,7 @@
       <c r="AK37" s="11">
         <v>24.39</v>
       </c>
-      <c r="AM37" s="75" t="s">
+      <c r="AM37" s="117" t="s">
         <v>42</v>
       </c>
       <c r="AN37" s="9">
@@ -5507,7 +6421,7 @@
       <c r="AE38" s="14">
         <v>21.45</v>
       </c>
-      <c r="AG38" s="74"/>
+      <c r="AG38" s="116"/>
       <c r="AH38" s="12">
         <v>24.21</v>
       </c>
@@ -5520,7 +6434,7 @@
       <c r="AK38" s="14">
         <v>21.45</v>
       </c>
-      <c r="AM38" s="75"/>
+      <c r="AM38" s="117"/>
       <c r="AN38" s="12">
         <v>24.21</v>
       </c>
@@ -5556,7 +6470,7 @@
       <c r="AE39" s="14">
         <v>32.74</v>
       </c>
-      <c r="AG39" s="74"/>
+      <c r="AG39" s="116"/>
       <c r="AH39" s="12">
         <v>26.88</v>
       </c>
@@ -5569,7 +6483,7 @@
       <c r="AK39" s="14">
         <v>32.74</v>
       </c>
-      <c r="AM39" s="75"/>
+      <c r="AM39" s="117"/>
       <c r="AN39" s="15">
         <v>26.88</v>
       </c>
@@ -5605,7 +6519,7 @@
       <c r="AE40" s="14">
         <v>24.21</v>
       </c>
-      <c r="AG40" s="74" t="s">
+      <c r="AG40" s="116" t="s">
         <v>43</v>
       </c>
       <c r="AH40" s="9">
@@ -5620,7 +6534,7 @@
       <c r="AK40" s="11">
         <v>24.21</v>
       </c>
-      <c r="AM40" s="75" t="s">
+      <c r="AM40" s="117" t="s">
         <v>43</v>
       </c>
       <c r="AN40" s="12">
@@ -5658,7 +6572,7 @@
       <c r="AE41" s="14">
         <v>25.67</v>
       </c>
-      <c r="AG41" s="74"/>
+      <c r="AG41" s="116"/>
       <c r="AH41" s="12">
         <v>23.4</v>
       </c>
@@ -5671,7 +6585,7 @@
       <c r="AK41" s="14">
         <v>25.67</v>
       </c>
-      <c r="AM41" s="75"/>
+      <c r="AM41" s="117"/>
       <c r="AN41" s="12">
         <v>23.4</v>
       </c>
@@ -5707,7 +6621,7 @@
       <c r="AE42" s="17">
         <v>23.42</v>
       </c>
-      <c r="AG42" s="74"/>
+      <c r="AG42" s="116"/>
       <c r="AH42" s="15">
         <v>23.35</v>
       </c>
@@ -5720,7 +6634,7 @@
       <c r="AK42" s="17">
         <v>23.42</v>
       </c>
-      <c r="AM42" s="75"/>
+      <c r="AM42" s="117"/>
       <c r="AN42" s="15">
         <v>23.35</v>
       </c>
@@ -6247,7 +7161,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:Y8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -6260,192 +7174,192 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:25" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="81" t="s">
+      <c r="B2" s="118" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="G2" s="81" t="s">
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="G2" s="118" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="L2" s="81" t="s">
-        <v>122</v>
-      </c>
-      <c r="M2" s="81"/>
-      <c r="N2" s="81"/>
-      <c r="O2" s="81"/>
-      <c r="Q2" s="86" t="s">
+      <c r="H2" s="118"/>
+      <c r="I2" s="118"/>
+      <c r="J2" s="118"/>
+      <c r="L2" s="118" t="s">
+        <v>120</v>
+      </c>
+      <c r="M2" s="118"/>
+      <c r="N2" s="118"/>
+      <c r="O2" s="118"/>
+      <c r="Q2" s="119" t="s">
         <v>49</v>
       </c>
-      <c r="R2" s="81"/>
-      <c r="S2" s="81"/>
-      <c r="T2" s="81"/>
-      <c r="V2" s="58" t="s">
+      <c r="R2" s="118"/>
+      <c r="S2" s="118"/>
+      <c r="T2" s="118"/>
+      <c r="V2" s="100" t="s">
         <v>48</v>
       </c>
-      <c r="W2" s="58"/>
-      <c r="X2" s="58"/>
-      <c r="Y2" s="58"/>
+      <c r="W2" s="100"/>
+      <c r="X2" s="100"/>
+      <c r="Y2" s="100"/>
     </row>
     <row r="3" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="76"/>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="83"/>
-      <c r="K3" s="82"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="79"/>
-      <c r="P3" s="82"/>
-      <c r="Q3" s="83"/>
-      <c r="R3" s="83"/>
-      <c r="S3" s="83"/>
-      <c r="T3" s="79"/>
-      <c r="V3" s="87"/>
-      <c r="W3" s="87"/>
-      <c r="X3" s="87"/>
-      <c r="Y3" s="87"/>
+      <c r="A3" s="57"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
+      <c r="O3" s="60"/>
+      <c r="P3" s="63"/>
+      <c r="Q3" s="64"/>
+      <c r="R3" s="64"/>
+      <c r="S3" s="64"/>
+      <c r="T3" s="60"/>
+      <c r="V3" s="67"/>
+      <c r="W3" s="67"/>
+      <c r="X3" s="67"/>
+      <c r="Y3" s="67"/>
     </row>
     <row r="4" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="76"/>
-      <c r="B4" s="53"/>
+      <c r="A4" s="57"/>
+      <c r="B4" s="52"/>
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
-      <c r="E4" s="79"/>
-      <c r="F4" s="82"/>
-      <c r="G4" s="84"/>
-      <c r="H4" s="84"/>
-      <c r="I4" s="84"/>
-      <c r="J4" s="84"/>
-      <c r="K4" s="82"/>
-      <c r="L4" s="53"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="63"/>
+      <c r="L4" s="52"/>
       <c r="M4" s="13"/>
       <c r="N4" s="13"/>
-      <c r="O4" s="79"/>
-      <c r="P4" s="82"/>
-      <c r="Q4" s="84"/>
-      <c r="R4" s="84"/>
-      <c r="S4" s="84"/>
-      <c r="T4" s="79"/>
-      <c r="V4" s="87"/>
-      <c r="W4" s="87"/>
-      <c r="X4" s="87"/>
-      <c r="Y4" s="87"/>
+      <c r="O4" s="60"/>
+      <c r="P4" s="63"/>
+      <c r="Q4" s="65"/>
+      <c r="R4" s="65"/>
+      <c r="S4" s="65"/>
+      <c r="T4" s="60"/>
+      <c r="V4" s="67"/>
+      <c r="W4" s="67"/>
+      <c r="X4" s="67"/>
+      <c r="Y4" s="67"/>
     </row>
     <row r="5" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="76"/>
-      <c r="B5" s="53"/>
+      <c r="A5" s="57"/>
+      <c r="B5" s="52"/>
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="82"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="84"/>
-      <c r="K5" s="82"/>
-      <c r="L5" s="77"/>
-      <c r="M5" s="78"/>
-      <c r="N5" s="78"/>
-      <c r="O5" s="80"/>
-      <c r="P5" s="82"/>
-      <c r="Q5" s="85"/>
-      <c r="R5" s="85"/>
-      <c r="S5" s="85"/>
-      <c r="T5" s="80"/>
-      <c r="V5" s="87"/>
-      <c r="W5" s="87"/>
-      <c r="X5" s="87"/>
-      <c r="Y5" s="87"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="63"/>
+      <c r="L5" s="58"/>
+      <c r="M5" s="59"/>
+      <c r="N5" s="59"/>
+      <c r="O5" s="61"/>
+      <c r="P5" s="63"/>
+      <c r="Q5" s="66"/>
+      <c r="R5" s="66"/>
+      <c r="S5" s="66"/>
+      <c r="T5" s="61"/>
+      <c r="V5" s="67"/>
+      <c r="W5" s="67"/>
+      <c r="X5" s="67"/>
+      <c r="Y5" s="67"/>
     </row>
     <row r="6" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="76"/>
-      <c r="B6" s="53"/>
+      <c r="A6" s="57"/>
+      <c r="B6" s="52"/>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="84"/>
-      <c r="H6" s="84"/>
-      <c r="I6" s="84"/>
-      <c r="J6" s="84"/>
-      <c r="K6" s="82"/>
-      <c r="L6" s="53"/>
-      <c r="M6" s="53"/>
-      <c r="N6" s="53"/>
-      <c r="O6" s="79"/>
-      <c r="P6" s="82"/>
-      <c r="Q6" s="84"/>
-      <c r="R6" s="84"/>
-      <c r="S6" s="84"/>
-      <c r="T6" s="79"/>
-      <c r="V6" s="87"/>
-      <c r="W6" s="87"/>
-      <c r="X6" s="87"/>
-      <c r="Y6" s="87"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="65"/>
+      <c r="I6" s="65"/>
+      <c r="J6" s="65"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="52"/>
+      <c r="M6" s="52"/>
+      <c r="N6" s="52"/>
+      <c r="O6" s="60"/>
+      <c r="P6" s="63"/>
+      <c r="Q6" s="65"/>
+      <c r="R6" s="65"/>
+      <c r="S6" s="65"/>
+      <c r="T6" s="60"/>
+      <c r="V6" s="67"/>
+      <c r="W6" s="67"/>
+      <c r="X6" s="67"/>
+      <c r="Y6" s="67"/>
     </row>
     <row r="7" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="76"/>
-      <c r="B7" s="53"/>
+      <c r="A7" s="57"/>
+      <c r="B7" s="52"/>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="84"/>
-      <c r="H7" s="84"/>
-      <c r="I7" s="84"/>
-      <c r="J7" s="84"/>
-      <c r="K7" s="82"/>
-      <c r="L7" s="53"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="65"/>
+      <c r="K7" s="63"/>
+      <c r="L7" s="52"/>
       <c r="M7" s="13"/>
       <c r="N7" s="13"/>
-      <c r="O7" s="79"/>
-      <c r="P7" s="82"/>
-      <c r="Q7" s="84"/>
-      <c r="R7" s="84"/>
-      <c r="S7" s="84"/>
-      <c r="T7" s="79"/>
-      <c r="V7" s="87"/>
-      <c r="W7" s="87"/>
-      <c r="X7" s="87"/>
-      <c r="Y7" s="87"/>
+      <c r="O7" s="60"/>
+      <c r="P7" s="63"/>
+      <c r="Q7" s="65"/>
+      <c r="R7" s="65"/>
+      <c r="S7" s="65"/>
+      <c r="T7" s="60"/>
+      <c r="V7" s="67"/>
+      <c r="W7" s="67"/>
+      <c r="X7" s="67"/>
+      <c r="Y7" s="67"/>
     </row>
     <row r="8" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="76"/>
-      <c r="B8" s="77"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="80"/>
-      <c r="F8" s="82"/>
-      <c r="G8" s="85"/>
-      <c r="H8" s="85"/>
-      <c r="I8" s="85"/>
-      <c r="J8" s="85"/>
-      <c r="K8" s="82"/>
-      <c r="L8" s="77"/>
-      <c r="M8" s="78"/>
-      <c r="N8" s="78"/>
-      <c r="O8" s="80"/>
-      <c r="P8" s="82"/>
-      <c r="Q8" s="85"/>
-      <c r="R8" s="85"/>
-      <c r="S8" s="85"/>
-      <c r="T8" s="80"/>
-      <c r="V8" s="87"/>
-      <c r="W8" s="87"/>
-      <c r="X8" s="87"/>
-      <c r="Y8" s="87"/>
+      <c r="A8" s="57"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="66"/>
+      <c r="H8" s="66"/>
+      <c r="I8" s="66"/>
+      <c r="J8" s="66"/>
+      <c r="K8" s="63"/>
+      <c r="L8" s="58"/>
+      <c r="M8" s="59"/>
+      <c r="N8" s="59"/>
+      <c r="O8" s="61"/>
+      <c r="P8" s="63"/>
+      <c r="Q8" s="66"/>
+      <c r="R8" s="66"/>
+      <c r="S8" s="66"/>
+      <c r="T8" s="61"/>
+      <c r="V8" s="67"/>
+      <c r="W8" s="67"/>
+      <c r="X8" s="67"/>
+      <c r="Y8" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -6458,4 +7372,104 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03B883F1-1F0C-4524-B73F-E7D1A0CFC916}">
+  <dimension ref="B2:X6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T13" sqref="T13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="18" width="9.140625" style="1"/>
+    <col min="19" max="19" width="7.140625" style="1" customWidth="1"/>
+    <col min="20" max="21" width="9.140625" style="1"/>
+    <col min="22" max="22" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.140625" style="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:24" ht="21" x14ac:dyDescent="0.35">
+      <c r="R2" s="78" t="s">
+        <v>132</v>
+      </c>
+      <c r="S2" s="78"/>
+      <c r="T2" s="78" t="s">
+        <v>133</v>
+      </c>
+      <c r="U2" s="78"/>
+      <c r="V2" s="78" t="s">
+        <v>134</v>
+      </c>
+      <c r="W2" s="78"/>
+      <c r="X2" s="79" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="2:24" ht="21" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="R3" s="78"/>
+      <c r="S3" s="78"/>
+      <c r="T3" s="78"/>
+      <c r="U3" s="78"/>
+      <c r="V3" s="78"/>
+      <c r="W3" s="78"/>
+      <c r="X3" s="78"/>
+    </row>
+    <row r="4" spans="2:24" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="R4" s="80" t="s">
+        <v>135</v>
+      </c>
+      <c r="S4" s="79"/>
+      <c r="T4" s="80" t="s">
+        <v>136</v>
+      </c>
+      <c r="U4" s="79"/>
+      <c r="V4" s="81" t="s">
+        <v>137</v>
+      </c>
+      <c r="W4" s="78"/>
+      <c r="X4" s="80">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:24" ht="21.75" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="R5" s="79" t="s">
+        <v>129</v>
+      </c>
+      <c r="S5" s="79"/>
+      <c r="T5" s="79" t="s">
+        <v>129</v>
+      </c>
+      <c r="U5" s="79"/>
+      <c r="V5" s="79" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="2:24" ht="21" x14ac:dyDescent="0.35">
+      <c r="R6" s="78"/>
+      <c r="S6" s="78"/>
+      <c r="T6" s="78"/>
+      <c r="U6" s="78"/>
+      <c r="V6" s="79" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>